<commit_message>
Update link for user function
</commit_message>
<xml_diff>
--- a/Thong ke Url.xlsx
+++ b/Thong ke Url.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>LINK JAPTOOL</t>
   </si>
@@ -39,18 +39,6 @@
     <t>User</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Đăng nhập user vào systems</t>
-  </si>
-  <si>
-    <t>Signin</t>
-  </si>
-  <si>
-    <t>Đăng ký user</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -58,13 +46,58 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>http://localhost:1337/japtool/auth</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>Đăng ký tài khoản mới</t>
+  </si>
+  <si>
+    <t>http://localhost:1337/japtool/forgotPassword.html</t>
+  </si>
+  <si>
+    <t>Forgot password</t>
+  </si>
+  <si>
+    <t>Lấy lại mật khẩu</t>
+  </si>
+  <si>
+    <t>http://localhost:1337/japtool/user/show/userID</t>
+  </si>
+  <si>
+    <t>User Profile</t>
+  </si>
+  <si>
+    <t>View user profile</t>
+  </si>
+  <si>
+    <t>Edit user profile</t>
+  </si>
+  <si>
+    <t>Change password</t>
+  </si>
+  <si>
+    <t>Change avatar</t>
+  </si>
+  <si>
+    <t>Friends function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +125,14 @@
       <b/>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,10 +302,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -277,12 +319,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -585,25 +629,25 @@
   <dimension ref="A2:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
@@ -620,79 +664,113 @@
       <c r="D5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>10</v>
+      <c r="E5" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -859,8 +937,12 @@
   <mergeCells count="1">
     <mergeCell ref="A2:D2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="66" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>